<commit_message>
cleaning and addition of LR
</commit_message>
<xml_diff>
--- a/data_descriptives_after_MICE.xlsx
+++ b/data_descriptives_after_MICE.xlsx
@@ -1435,7 +1435,7 @@
         <v>0.4933</v>
       </c>
       <c r="AV3" t="n">
-        <v>-0.06539592609485528</v>
+        <v>-0.06834955435453159</v>
       </c>
       <c r="AW3" t="n">
         <v>0</v>
@@ -1447,10 +1447,10 @@
         <v>0</v>
       </c>
       <c r="AZ3" t="n">
-        <v>-0.0033358121513448</v>
+        <v>0</v>
       </c>
       <c r="BA3" t="n">
-        <v>-0.01980249800050752</v>
+        <v>-0.01048984217249318</v>
       </c>
       <c r="BB3" t="n">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="BE3" t="n">
-        <v>-0.06417665014767916</v>
+        <v>-0.06346346529129036</v>
       </c>
       <c r="BF3" t="n">
         <v>0</v>
@@ -1474,10 +1474,10 @@
         <v>0</v>
       </c>
       <c r="BI3" t="n">
-        <v>-0.003705560144293608</v>
+        <v>0</v>
       </c>
       <c r="BJ3" t="n">
-        <v>-0.02256204854913135</v>
+        <v>-0.01350133615972497</v>
       </c>
       <c r="BK3" t="n">
         <v>0</v>
@@ -1489,7 +1489,7 @@
         <v>0.4933</v>
       </c>
       <c r="BN3" t="n">
-        <v>-0.06560044003048214</v>
+        <v>-0.06914825245171299</v>
       </c>
       <c r="BO3" t="n">
         <v>0</v>
@@ -1501,10 +1501,10 @@
         <v>0</v>
       </c>
       <c r="BR3" t="n">
-        <v>-0.003348741753291216</v>
+        <v>0</v>
       </c>
       <c r="BS3" t="n">
-        <v>-0.02075548249447042</v>
+        <v>-0.01149420626780502</v>
       </c>
       <c r="BT3" t="n">
         <v>1</v>
@@ -1531,7 +1531,7 @@
         <v>0</v>
       </c>
       <c r="CB3" t="n">
-        <v>0</v>
+        <v>-0.0008498064264525762</v>
       </c>
       <c r="CC3" t="n">
         <v>-3409</v>
@@ -1597,13 +1597,13 @@
         <v>0</v>
       </c>
       <c r="CX3" t="n">
-        <v>-0.03231060712597356</v>
+        <v>-0.02589212009742492</v>
       </c>
       <c r="CY3" t="n">
-        <v>-0.01991224008883125</v>
+        <v>-0.007585994751205218</v>
       </c>
       <c r="CZ3" t="n">
-        <v>-0.04481283971176839</v>
+        <v>0</v>
       </c>
       <c r="DA3" t="n">
         <v>0</v>
@@ -1977,7 +1977,7 @@
         <v>10905.51803154506</v>
       </c>
       <c r="L5" t="n">
-        <v>281335.4764871668</v>
+        <v>281336.94137175</v>
       </c>
       <c r="M5" t="n">
         <v>0.4873902931960989</v>
@@ -2067,94 +2067,94 @@
         <v>8.056186316446576</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.09345422050453633</v>
+        <v>0.103173098434489</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.1620061371960804</v>
+        <v>0.1620134241373689</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.1371100026676574</v>
+        <v>0.1326312370746145</v>
       </c>
       <c r="AS5" t="n">
-        <v>0.0426804156765106</v>
+        <v>0.04202660262247519</v>
       </c>
       <c r="AT5" t="n">
-        <v>0.02511401051036344</v>
+        <v>0.02598690690414279</v>
       </c>
       <c r="AU5" t="n">
-        <v>0.0047356670281306</v>
+        <v>0.004546482354745358</v>
       </c>
       <c r="AV5" t="n">
-        <v>0.05545187131686675</v>
+        <v>0.0561659616600887</v>
       </c>
       <c r="AW5" t="n">
-        <v>0.03362297502345808</v>
+        <v>0.03246848306892767</v>
       </c>
       <c r="AX5" t="n">
-        <v>0.06786331337249606</v>
+        <v>0.07147750213957864</v>
       </c>
       <c r="AY5" t="n">
-        <v>0.02430242604499511</v>
+        <v>0.02435248903068241</v>
       </c>
       <c r="AZ5" t="n">
-        <v>0.04292250061578647</v>
+        <v>0.0428438280422095</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.02050728529859988</v>
+        <v>0.02127519230028399</v>
       </c>
       <c r="BB5" t="n">
-        <v>0.04196413895982266</v>
+        <v>0.03994782635701525</v>
       </c>
       <c r="BC5" t="n">
-        <v>0.02698199900722202</v>
+        <v>0.02649496179872661</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.006836340012212502</v>
+        <v>0.006428064423120565</v>
       </c>
       <c r="BE5" t="n">
-        <v>0.05338552303757681</v>
+        <v>0.0536987082513803</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.03406798214974738</v>
+        <v>0.03323001182290512</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.06743486095838681</v>
+        <v>0.06866222409854451</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.02462083144951041</v>
+        <v>0.02470944814757399</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.04402185729649342</v>
+        <v>0.04277051884462714</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.02177833709935093</v>
+        <v>0.02207955549375783</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.04293295926089027</v>
+        <v>0.04119123823787647</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.02508723448704391</v>
+        <v>0.02525954850203326</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.004370393142379997</v>
+        <v>0.004334972861881025</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.05514103274301558</v>
+        <v>0.05574637722610173</v>
       </c>
       <c r="BO5" t="n">
-        <v>0.03374419183465525</v>
+        <v>0.03281560254581525</v>
       </c>
       <c r="BP5" t="n">
-        <v>0.06794177783912951</v>
+        <v>0.07107233374979242</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.02459888068722061</v>
+        <v>0.0246067353789282</v>
       </c>
       <c r="BR5" t="n">
-        <v>0.04353263932472187</v>
+        <v>0.04297030232282382</v>
       </c>
       <c r="BS5" t="n">
-        <v>0.02106902256345789</v>
+        <v>0.02184627511891423</v>
       </c>
       <c r="BT5" t="n">
         <v>0.4427009592174757</v>
@@ -2163,25 +2163,25 @@
         <v>0.5110636161687213</v>
       </c>
       <c r="BV5" t="n">
-        <v>0.04362748814194724</v>
+        <v>0.04387625478466212</v>
       </c>
       <c r="BW5" t="n">
         <v>0.8939870801732662</v>
       </c>
       <c r="BX5" t="n">
-        <v>0.01056637011981041</v>
+        <v>0.01098508208894688</v>
       </c>
       <c r="BY5" t="n">
-        <v>1.551133474176228</v>
+        <v>1.551183090186825</v>
       </c>
       <c r="BZ5" t="n">
-        <v>0.2251876614055778</v>
+        <v>0.2251971447103978</v>
       </c>
       <c r="CA5" t="n">
-        <v>1.537173061500536</v>
+        <v>1.537213581130476</v>
       </c>
       <c r="CB5" t="n">
-        <v>0.1608960995166978</v>
+        <v>0.1609030712433077</v>
       </c>
       <c r="CC5" t="n">
         <v>706.7895102309517</v>
@@ -2247,22 +2247,22 @@
         <v>0</v>
       </c>
       <c r="CX5" t="n">
-        <v>0.01658176947087402</v>
+        <v>0.01649981738486565</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.01262961862626101</v>
+        <v>0.01232115011941043</v>
       </c>
       <c r="CZ5" t="n">
-        <v>0.06121258230929773</v>
+        <v>0.0610565643784701</v>
       </c>
       <c r="DA5" t="n">
-        <v>0.3456532939470125</v>
+        <v>0.3470901431481323</v>
       </c>
       <c r="DB5" t="n">
-        <v>0.394913960540595</v>
+        <v>0.3970634181197694</v>
       </c>
       <c r="DC5" t="n">
-        <v>1.28394408740761</v>
+        <v>1.283851118541529</v>
       </c>
     </row>
     <row r="6">
@@ -2302,7 +2302,7 @@
         <v>27120.71621621622</v>
       </c>
       <c r="L6" t="n">
-        <v>535628.7822254505</v>
+        <v>535627.0019095155</v>
       </c>
       <c r="M6" t="n">
         <v>1.301301301301301</v>
@@ -2392,94 +2392,94 @@
         <v>10.77677677677678</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.4969296756723959</v>
+        <v>0.4969604033047024</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.5155526389841133</v>
+        <v>0.5155465927595724</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.5131108755702763</v>
+        <v>0.5130559177684323</v>
       </c>
       <c r="AS6" t="n">
-        <v>0.09742530231664757</v>
+        <v>0.09904420824242778</v>
       </c>
       <c r="AT6" t="n">
-        <v>0.08042006635482385</v>
+        <v>0.07778123016219282</v>
       </c>
       <c r="AU6" t="n">
-        <v>0.9801666266090441</v>
+        <v>0.9803599790578759</v>
       </c>
       <c r="AV6" t="n">
-        <v>0.0572920435702709</v>
+        <v>0.05449563262391398</v>
       </c>
       <c r="AW6" t="n">
-        <v>0.1372654411890173</v>
+        <v>0.1396392754666966</v>
       </c>
       <c r="AX6" t="n">
-        <v>0.2156282485053171</v>
+        <v>0.2038560643924456</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.05841864683287033</v>
+        <v>0.05803675588273972</v>
       </c>
       <c r="AZ6" t="n">
-        <v>0.08892125343599695</v>
+        <v>0.08881311245039997</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.02582062115237005</v>
+        <v>0.02165919305182338</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.09419900919418898</v>
+        <v>0.09899013204910595</v>
       </c>
       <c r="BC6" t="n">
-        <v>0.07700540633128049</v>
+        <v>0.07781667858776187</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.9778918297269602</v>
+        <v>0.9790350228377188</v>
       </c>
       <c r="BE6" t="n">
-        <v>0.05400302276376447</v>
+        <v>0.05232357591105089</v>
       </c>
       <c r="BF6" t="n">
-        <v>0.1343308211634946</v>
+        <v>0.1347167893108235</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.2121553766738887</v>
+        <v>0.2081997699272716</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.05787510744097391</v>
+        <v>0.05751976539683133</v>
       </c>
       <c r="BI6" t="n">
-        <v>0.08510819925126885</v>
+        <v>0.08759615952415677</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.02402679860236656</v>
+        <v>0.02117567457511895</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.09792336338570859</v>
+        <v>0.1015886278086519</v>
       </c>
       <c r="BL6" t="n">
-        <v>0.08005354227328855</v>
+        <v>0.07888757077532256</v>
       </c>
       <c r="BM6" t="n">
-        <v>0.9809952783368121</v>
+        <v>0.9807784471780124</v>
       </c>
       <c r="BN6" t="n">
-        <v>0.05705928843339852</v>
+        <v>0.05536661078171171</v>
       </c>
       <c r="BO6" t="n">
-        <v>0.1377872887248031</v>
+        <v>0.1396596698386499</v>
       </c>
       <c r="BP6" t="n">
-        <v>0.2154830020638937</v>
+        <v>0.2050253433611077</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.05912755846079432</v>
+        <v>0.05883633615191687</v>
       </c>
       <c r="BR6" t="n">
-        <v>0.09058382623960914</v>
+        <v>0.09157084500895245</v>
       </c>
       <c r="BS6" t="n">
-        <v>0.02605612890170289</v>
+        <v>0.02177042348978891</v>
       </c>
       <c r="BT6" t="n">
         <v>1.898898898898899</v>
@@ -2488,25 +2488,25 @@
         <v>1.503503503503504</v>
       </c>
       <c r="BV6" t="n">
-        <v>0.08658199177967109</v>
+        <v>0.08590109189150916</v>
       </c>
       <c r="BW6" t="n">
         <v>2.827827827827828</v>
       </c>
       <c r="BX6" t="n">
-        <v>0.009850090212539186</v>
+        <v>0.009609004169864481</v>
       </c>
       <c r="BY6" t="n">
-        <v>1.30650658147113</v>
+        <v>1.306417433279428</v>
       </c>
       <c r="BZ6" t="n">
-        <v>0.126343580634709</v>
+        <v>0.1262993104407133</v>
       </c>
       <c r="CA6" t="n">
-        <v>1.2894659053447</v>
+        <v>1.289392838358581</v>
       </c>
       <c r="CB6" t="n">
-        <v>0.08726839857117651</v>
+        <v>0.08722257781536563</v>
       </c>
       <c r="CC6" t="n">
         <v>-979.7657657657658</v>
@@ -2572,22 +2572,22 @@
         <v>0</v>
       </c>
       <c r="CX6" t="n">
-        <v>0.009045216099395263</v>
+        <v>0.009051893742401791</v>
       </c>
       <c r="CY6" t="n">
-        <v>0.007032782977960513</v>
+        <v>0.006976538998277805</v>
       </c>
       <c r="CZ6" t="n">
-        <v>0.03588052082366906</v>
+        <v>0.0361121418681964</v>
       </c>
       <c r="DA6" t="n">
-        <v>0.2294077681272599</v>
+        <v>0.2312730809530294</v>
       </c>
       <c r="DB6" t="n">
-        <v>0.2912005705436816</v>
+        <v>0.291522785768328</v>
       </c>
       <c r="DC6" t="n">
-        <v>1.902234060384413</v>
+        <v>1.902287474159097</v>
       </c>
     </row>
     <row r="7">
@@ -2717,94 +2717,94 @@
         <v>8</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.493554752800681</v>
+        <v>0.4955623721707529</v>
       </c>
       <c r="AQ7" t="n">
         <v>0.5711913307583379</v>
       </c>
       <c r="AR7" t="n">
-        <v>0.5238928463634924</v>
+        <v>0.5130360317720301</v>
       </c>
       <c r="AS7" t="n">
-        <v>0.08152765707098601</v>
+        <v>0.08385812800130335</v>
       </c>
       <c r="AT7" t="n">
-        <v>0.07742847813751645</v>
+        <v>0.07221450703691004</v>
       </c>
       <c r="AU7" t="n">
-        <v>0.9806378037068308</v>
+        <v>0.9808384293699252</v>
       </c>
       <c r="AV7" t="n">
-        <v>0.0379961694274364</v>
+        <v>0.0324771139014379</v>
       </c>
       <c r="AW7" t="n">
-        <v>0.1325796221844858</v>
+        <v>0.1379</v>
       </c>
       <c r="AX7" t="n">
-        <v>0.1980501831995663</v>
+        <v>0.1739708279247994</v>
       </c>
       <c r="AY7" t="n">
-        <v>0.0531354716365721</v>
+        <v>0.05234270711431947</v>
       </c>
       <c r="AZ7" t="n">
-        <v>0.07275608269423975</v>
+        <v>0.07229327079430101</v>
       </c>
       <c r="BA7" t="n">
-        <v>0.02076987387953371</v>
+        <v>0.01256745275660578</v>
       </c>
       <c r="BB7" t="n">
-        <v>0.07832255590774582</v>
+        <v>0.08742236473856652</v>
       </c>
       <c r="BC7" t="n">
-        <v>0.07157093736262345</v>
+        <v>0.0729217898938159</v>
       </c>
       <c r="BD7" t="n">
-        <v>0.9793521514333159</v>
+        <v>0.9807362704447131</v>
       </c>
       <c r="BE7" t="n">
-        <v>0.03535986182703076</v>
+        <v>0.03202242077805297</v>
       </c>
       <c r="BF7" t="n">
-        <v>0.1315779256506224</v>
+        <v>0.1327474664384867</v>
       </c>
       <c r="BG7" t="n">
-        <v>0.1941963505077127</v>
+        <v>0.184857666396061</v>
       </c>
       <c r="BH7" t="n">
-        <v>0.05270987528251594</v>
+        <v>0.05188404032611363</v>
       </c>
       <c r="BI7" t="n">
-        <v>0.06688760104086057</v>
+        <v>0.07143272014100209</v>
       </c>
       <c r="BJ7" t="n">
-        <v>0.01720474146835529</v>
+        <v>0.01194563815547413</v>
       </c>
       <c r="BK7" t="n">
-        <v>0.08195401041465843</v>
+        <v>0.08829458792488301</v>
       </c>
       <c r="BL7" t="n">
-        <v>0.07699951019230017</v>
+        <v>0.07486981573233652</v>
       </c>
       <c r="BM7" t="n">
-        <v>0.9816</v>
+        <v>0.9811220535802468</v>
       </c>
       <c r="BN7" t="n">
-        <v>0.038180538641348</v>
+        <v>0.03365596965556104</v>
       </c>
       <c r="BO7" t="n">
-        <v>0.1340451279280731</v>
+        <v>0.1379</v>
       </c>
       <c r="BP7" t="n">
-        <v>0.1977983695855003</v>
+        <v>0.1764406694175532</v>
       </c>
       <c r="BQ7" t="n">
-        <v>0.05383157013675635</v>
+        <v>0.05327858031580367</v>
       </c>
       <c r="BR7" t="n">
-        <v>0.07454705763316999</v>
+        <v>0.07585494157496497</v>
       </c>
       <c r="BS7" t="n">
-        <v>0.02078019533076111</v>
+        <v>0.01240064718688126</v>
       </c>
       <c r="BT7" t="n">
         <v>2</v>
@@ -2813,7 +2813,7 @@
         <v>1</v>
       </c>
       <c r="BV7" t="n">
-        <v>0.07060911449140167</v>
+        <v>0.06894036018385516</v>
       </c>
       <c r="BW7" t="n">
         <v>3</v>
@@ -2912,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="DC7" t="n">
-        <v>1.800286521882645</v>
+        <v>1.800110952098913</v>
       </c>
     </row>
     <row r="8">
@@ -2952,7 +2952,7 @@
         <v>204091945.8710394</v>
       </c>
       <c r="L8" t="n">
-        <v>129498780339.2052</v>
+        <v>129500298202.5096</v>
       </c>
       <c r="M8" t="n">
         <v>0.6576235554191466</v>
@@ -3042,94 +3042,94 @@
         <v>117.6244701615443</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.0201537796342468</v>
+        <v>0.02128181719081568</v>
       </c>
       <c r="AQ8" t="n">
-        <v>0.0382855202409567</v>
+        <v>0.03828590951330329</v>
       </c>
       <c r="AR8" t="n">
-        <v>0.03189179931358525</v>
+        <v>0.03163243250163777</v>
       </c>
       <c r="AS8" t="n">
-        <v>0.005426682721352312</v>
+        <v>0.005364212887409809</v>
       </c>
       <c r="AT8" t="n">
-        <v>0.002271563056699643</v>
+        <v>0.002291191358480511</v>
       </c>
       <c r="AU8" t="n">
-        <v>0.0003911484763875598</v>
+        <v>0.0003908150210877011</v>
       </c>
       <c r="AV8" t="n">
-        <v>0.009093416276228084</v>
+        <v>0.009143146773307144</v>
       </c>
       <c r="AW8" t="n">
-        <v>0.003785216174869286</v>
+        <v>0.003754259483012278</v>
       </c>
       <c r="AX8" t="n">
-        <v>0.01170403421358328</v>
+        <v>0.01209640701351525</v>
       </c>
       <c r="AY8" t="n">
-        <v>0.002493106987688535</v>
+        <v>0.002503449475820893</v>
       </c>
       <c r="AZ8" t="n">
-        <v>0.006113193174163557</v>
+        <v>0.006086096109210615</v>
       </c>
       <c r="BA8" t="n">
-        <v>0.002681132173287295</v>
+        <v>0.002707541416401497</v>
       </c>
       <c r="BB8" t="n">
-        <v>0.005382927204630151</v>
+        <v>0.005215403409720813</v>
       </c>
       <c r="BC8" t="n">
-        <v>0.002497208255284519</v>
+        <v>0.00246951855259184</v>
       </c>
       <c r="BD8" t="n">
-        <v>0.001973024087726126</v>
+        <v>0.001971500763427782</v>
       </c>
       <c r="BE8" t="n">
-        <v>0.008777657260539192</v>
+        <v>0.008784988176392033</v>
       </c>
       <c r="BF8" t="n">
-        <v>0.003876676824004147</v>
+        <v>0.003858425684357852</v>
       </c>
       <c r="BG8" t="n">
-        <v>0.01166981627013722</v>
+        <v>0.01179196432732534</v>
       </c>
       <c r="BH8" t="n">
-        <v>0.002605901105156502</v>
+        <v>0.002615620401613208</v>
       </c>
       <c r="BI8" t="n">
-        <v>0.006530030954780247</v>
+        <v>0.006386861710499212</v>
       </c>
       <c r="BJ8" t="n">
-        <v>0.003020295679598822</v>
+        <v>0.003032183417102996</v>
       </c>
       <c r="BK8" t="n">
-        <v>0.005529591697611596</v>
+        <v>0.005375313772722254</v>
       </c>
       <c r="BL8" t="n">
-        <v>0.002267940105062</v>
+        <v>0.002270937091724466</v>
       </c>
       <c r="BM8" t="n">
-        <v>0.0002856125017443356</v>
+        <v>0.0002847780332430891</v>
       </c>
       <c r="BN8" t="n">
-        <v>0.009054726416535286</v>
+        <v>0.009112873498313591</v>
       </c>
       <c r="BO8" t="n">
-        <v>0.003822258152412831</v>
+        <v>0.003794356635281106</v>
       </c>
       <c r="BP8" t="n">
-        <v>0.0117486252391897</v>
+        <v>0.01207902652541699</v>
       </c>
       <c r="BQ8" t="n">
-        <v>0.002570689416001277</v>
+        <v>0.002580082053191583</v>
       </c>
       <c r="BR8" t="n">
-        <v>0.006331969770293029</v>
+        <v>0.006268185437733821</v>
       </c>
       <c r="BS8" t="n">
-        <v>0.002807498280604008</v>
+        <v>0.00283617294121849</v>
       </c>
       <c r="BT8" t="n">
         <v>0.5518925739366622</v>
@@ -3138,25 +3138,25 @@
         <v>0.2802983344065508</v>
       </c>
       <c r="BV8" t="n">
-        <v>0.006159322573669338</v>
+        <v>0.006174640654042887</v>
       </c>
       <c r="BW8" t="n">
         <v>1.531449284956299</v>
       </c>
       <c r="BX8" t="n">
-        <v>0.004965896235842143</v>
+        <v>0.004970142988546125</v>
       </c>
       <c r="BY8" t="n">
-        <v>4.811381630146205</v>
+        <v>4.811606754842686</v>
       </c>
       <c r="BZ8" t="n">
-        <v>0.1563794768298806</v>
+        <v>0.1563874698473492</v>
       </c>
       <c r="CA8" t="n">
-        <v>4.724398028728417</v>
+        <v>4.724581178153104</v>
       </c>
       <c r="CB8" t="n">
-        <v>0.1036084098315038</v>
+        <v>0.1036160498354396</v>
       </c>
       <c r="CC8" t="n">
         <v>692753.2276444782</v>
@@ -3222,22 +3222,22 @@
         <v>0</v>
       </c>
       <c r="CX8" t="n">
-        <v>0.007957002392093781</v>
+        <v>0.007954677340277362</v>
       </c>
       <c r="CY8" t="n">
-        <v>0.01199079778264057</v>
+        <v>0.01198404209740771</v>
       </c>
       <c r="CZ8" t="n">
-        <v>0.03599423955331532</v>
+        <v>0.03597030699899115</v>
       </c>
       <c r="DA8" t="n">
-        <v>0.4841130747828291</v>
+        <v>0.4844132396024792</v>
       </c>
       <c r="DB8" t="n">
-        <v>0.3612071315102596</v>
+        <v>0.361275899296724</v>
       </c>
       <c r="DC8" t="n">
-        <v>3.108713562241261</v>
+        <v>3.108681222546991</v>
       </c>
     </row>
     <row r="9">
@@ -3277,7 +3277,7 @@
         <v>14286.07524378335</v>
       </c>
       <c r="L9" t="n">
-        <v>359859.3896776979</v>
+        <v>359861.4986387258</v>
       </c>
       <c r="M9" t="n">
         <v>0.810939920967729</v>
@@ -3367,94 +3367,94 @@
         <v>10.84548155507833</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.141964008235351</v>
+        <v>0.1458828886155456</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.1956668603544215</v>
+        <v>0.1956678550843323</v>
       </c>
       <c r="AR9" t="n">
-        <v>0.1785827520047366</v>
+        <v>0.1778550884895841</v>
       </c>
       <c r="AS9" t="n">
-        <v>0.07366602148448301</v>
+        <v>0.07324078704799539</v>
       </c>
       <c r="AT9" t="n">
-        <v>0.04766091749745952</v>
+        <v>0.0478663906982813</v>
       </c>
       <c r="AU9" t="n">
-        <v>0.01977747396376898</v>
+        <v>0.01976904198709945</v>
       </c>
       <c r="AV9" t="n">
-        <v>0.09535940580890846</v>
+        <v>0.09561980324863226</v>
       </c>
       <c r="AW9" t="n">
-        <v>0.06152411051668513</v>
+        <v>0.06127201223244001</v>
       </c>
       <c r="AX9" t="n">
-        <v>0.1081851848155896</v>
+        <v>0.1099836670306789</v>
       </c>
       <c r="AY9" t="n">
-        <v>0.04993102229765114</v>
+        <v>0.0500344828675274</v>
       </c>
       <c r="AZ9" t="n">
-        <v>0.07818691178300596</v>
+        <v>0.07801343544038176</v>
       </c>
       <c r="BA9" t="n">
-        <v>0.05177965018506107</v>
+        <v>0.05203404093861534</v>
       </c>
       <c r="BB9" t="n">
-        <v>0.07336843466116849</v>
+        <v>0.0722177499630168</v>
       </c>
       <c r="BC9" t="n">
-        <v>0.04997207475465192</v>
+        <v>0.04969425069957127</v>
       </c>
       <c r="BD9" t="n">
-        <v>0.04441873577361389</v>
+        <v>0.04440158514544026</v>
       </c>
       <c r="BE9" t="n">
-        <v>0.09368915230985492</v>
+        <v>0.09372826775520837</v>
       </c>
       <c r="BF9" t="n">
-        <v>0.06226296510771188</v>
+        <v>0.06211622722250485</v>
       </c>
       <c r="BG9" t="n">
-        <v>0.1080269238205792</v>
+        <v>0.1085908114313791</v>
       </c>
       <c r="BH9" t="n">
-        <v>0.0510480274364887</v>
+        <v>0.05114313640766675</v>
       </c>
       <c r="BI9" t="n">
-        <v>0.08080860693503042</v>
+        <v>0.07991784350505969</v>
       </c>
       <c r="BJ9" t="n">
-        <v>0.05495721681088683</v>
+        <v>0.05506526506885258</v>
       </c>
       <c r="BK9" t="n">
-        <v>0.0743612244224878</v>
+        <v>0.07331653137405134</v>
       </c>
       <c r="BL9" t="n">
-        <v>0.04762289475726985</v>
+        <v>0.04765435018678218</v>
       </c>
       <c r="BM9" t="n">
-        <v>0.01690007401594252</v>
+        <v>0.0168753676476422</v>
       </c>
       <c r="BN9" t="n">
-        <v>0.09515632620343897</v>
+        <v>0.09546137176006633</v>
       </c>
       <c r="BO9" t="n">
-        <v>0.06182441388652893</v>
+        <v>0.06159834929022941</v>
       </c>
       <c r="BP9" t="n">
-        <v>0.1083910754591433</v>
+        <v>0.1099046246771126</v>
       </c>
       <c r="BQ9" t="n">
-        <v>0.05070196658909078</v>
+        <v>0.05079450810069513</v>
       </c>
       <c r="BR9" t="n">
-        <v>0.07957367510862515</v>
+        <v>0.07917187276889326</v>
       </c>
       <c r="BS9" t="n">
-        <v>0.05298583094190378</v>
+        <v>0.05325573153397192</v>
       </c>
       <c r="BT9" t="n">
         <v>0.7428947260121466</v>
@@ -3463,25 +3463,25 @@
         <v>0.5294320866801999</v>
       </c>
       <c r="BV9" t="n">
-        <v>0.07848135175740373</v>
+        <v>0.07857888173067168</v>
       </c>
       <c r="BW9" t="n">
         <v>1.237517387738976</v>
       </c>
       <c r="BX9" t="n">
-        <v>0.07046911547509407</v>
+        <v>0.07049924104943348</v>
       </c>
       <c r="BY9" t="n">
-        <v>2.193486181890874</v>
+        <v>2.193537497934031</v>
       </c>
       <c r="BZ9" t="n">
-        <v>0.3954484502812985</v>
+        <v>0.3954585564219709</v>
       </c>
       <c r="CA9" t="n">
-        <v>2.173568040970518</v>
+        <v>2.17361017161613</v>
       </c>
       <c r="CB9" t="n">
-        <v>0.321882602561095</v>
+        <v>0.3218944700292932</v>
       </c>
       <c r="CC9" t="n">
         <v>832.3179846936375</v>
@@ -3547,22 +3547,22 @@
         <v>0</v>
       </c>
       <c r="CX9" t="n">
-        <v>0.08920203132268782</v>
+        <v>0.08918899786564126</v>
       </c>
       <c r="CY9" t="n">
-        <v>0.1095025012620286</v>
+        <v>0.1094716497427882</v>
       </c>
       <c r="CZ9" t="n">
-        <v>0.1897214788929164</v>
+        <v>0.1896583955404852</v>
       </c>
       <c r="DA9" t="n">
-        <v>0.6957823472773861</v>
+        <v>0.6959980169529789</v>
       </c>
       <c r="DB9" t="n">
-        <v>0.6010051010684182</v>
+        <v>0.6010623089969326</v>
       </c>
       <c r="DC9" t="n">
-        <v>1.763154435164787</v>
+        <v>1.763145264164865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>